<commit_message>
Analyse de la répartition du temps de travail II
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Adrien/RepartitionDuTravail.xlsx
+++ b/Dossiers personnels/Adrien/RepartitionDuTravail.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRepos\PRO\BlaajjPaint\Dossiers personnels\Adrien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CA4129-CD3B-4085-93DF-23DB54163849}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDF0B9E-AF12-4844-B159-CED2D7C2D120}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="27840" windowHeight="12810" xr2:uid="{B17E6258-D8B2-42DC-B5D5-71953BBB4CE2}"/>
+    <workbookView xWindow="1920" yWindow="0" windowWidth="27840" windowHeight="12810" xr2:uid="{B17E6258-D8B2-42DC-B5D5-71953BBB4CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Planification</t>
   </si>
@@ -63,10 +63,22 @@
     <t>total</t>
   </si>
   <si>
-    <t>Réalisé</t>
-  </si>
-  <si>
     <t>Adrien</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Antoine</t>
+  </si>
+  <si>
+    <t>Loyse</t>
+  </si>
+  <si>
+    <t>Jérémie</t>
   </si>
 </sst>
 </file>
@@ -418,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F8C461-AEC7-42D9-8836-0E7559C825FE}">
-  <dimension ref="B3:E15"/>
+  <dimension ref="B3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,18 +442,30 @@
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -449,12 +473,32 @@
         <f>21.5+47</f>
         <v>68.5</v>
       </c>
+      <c r="D4">
+        <f>SUM(E4:J4)</f>
+        <v>77.75</v>
+      </c>
       <c r="E4">
         <f>3+1+1+5+1+1.5+2+2+1</f>
         <v>17.5</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>11+1.5+1.5</f>
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <f>10.5+3.5+1.5+1.5+1.5</f>
+        <v>18.5</v>
+      </c>
+      <c r="H4">
+        <f>4.75+3+1.5</f>
+        <v>9.25</v>
+      </c>
+      <c r="I4">
+        <f>12.5+3+3</f>
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -462,12 +506,32 @@
         <f>(8*3)</f>
         <v>24</v>
       </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D13" si="0">SUM(E5:J5)</f>
+        <v>49</v>
+      </c>
       <c r="E5">
         <f>5+2</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f>4+4</f>
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <f>6+3</f>
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <f>9+1.5+1.5</f>
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <f>10+3</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -475,12 +539,31 @@
         <f>(3*8)+(6*3)</f>
         <v>42</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>53.5</v>
+      </c>
       <c r="E6">
         <f>5+2.5+4</f>
         <v>11.5</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>8+4</f>
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <f>12+8</f>
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <f>6+4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -488,8 +571,29 @@
         <f>(3*4)+(6*3)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>6+5+5.5+1.5</f>
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <f>4+2+3</f>
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -497,8 +601,28 @@
         <f>(3*4)+(6*3)+(12.5)</f>
         <v>42.5</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>23.5</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>18.5+5</f>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -506,12 +630,29 @@
         <f>(47)+31</f>
         <v>78</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
       <c r="E9">
         <f>5+ 13+10</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -519,23 +660,61 @@
         <f>34+37+7</f>
         <v>78</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
       <c r="E10">
         <f>4+2+2</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>0.5+36.5+1</f>
+        <v>38</v>
+      </c>
+      <c r="G10">
+        <f>5+1+12+10+12+3+7</f>
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <f>9+13+10</f>
+        <v>32</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11">
         <v>41.5</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>61.5</v>
+      </c>
       <c r="E11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>5.5</v>
+      </c>
+      <c r="G11">
+        <f>3+6</f>
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <f>16</f>
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <f>21</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -543,11 +722,29 @@
         <f>13+36+5.5</f>
         <v>54.5</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>14.25</v>
+      </c>
       <c r="E12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f>0.5+4.5</f>
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>0.25</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -555,8 +752,27 @@
         <f>36+33+9</f>
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -567,6 +783,26 @@
       <c r="E15">
         <f>SUM(E4:E13)</f>
         <v>89</v>
+      </c>
+      <c r="F15">
+        <f>SUM(F4:F13)</f>
+        <v>96.5</v>
+      </c>
+      <c r="G15">
+        <f>SUM(G4:G13)</f>
+        <v>112.5</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:I15" si="1">SUM(H4:H13)</f>
+        <v>89.5</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="J15">
+        <f>SUM(J4:J13)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>